<commit_message>
1. add start_date and end_date for course 2. add test mail for admin 3. don't send mail if course still open
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>course_id</t>
   </si>
@@ -62,19 +62,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>course_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>為公司把把脈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Python 與資料科學入門</t>
+  </si>
+  <si>
+    <t>start time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>DYUx/dyu10401/201511</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>course_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>為公司把把脈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Python 與資料科學入門</t>
+    <t>course-v1:FCUx+QA76+19004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017/01/01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/02/01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/08/01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>test@hotmail.com</t>
@@ -143,7 +167,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -430,7 +454,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -439,8 +463,8 @@
     <col min="3" max="3" width="26.875" customWidth="1"/>
     <col min="4" max="4" width="16.125" customWidth="1"/>
     <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="12.25" customWidth="1"/>
-    <col min="7" max="7" width="20.25" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -451,13 +475,19 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -468,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -476,37 +506,45 @@
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -514,8 +552,12 @@
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>

</xml_diff>

<commit_message>
add more insights informations
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">課程代碼</t>
   </si>
@@ -81,12 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">2022-02-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test@hotmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">C02</t>
@@ -292,20 +286,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2212765957447"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.7191489361702"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1787234042553"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.6893617021277"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.2595744680851"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.00851063829787"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.6978723404255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.8553191489362"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.531914893617"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.8297872340426"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0127659574468"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.8340425531915"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.00851063829787"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,55 +352,31 @@
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="gyli@mail.fcu.edu.tw"/>
-    <hyperlink ref="E3" r:id="rId2" display="test@hotmail.com"/>
-    <hyperlink ref="E4" r:id="rId3" display="gyli@mail.fcu.edu.tw"/>
+    <hyperlink ref="E3" r:id="rId2" display="gyli@mail.fcu.edu.tw"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>